<commit_message>
Nachträglicher Upload von Änderungen - ein Teil der vorherig verwendeten ChatGPT-Datei war doppelt in full_df enthalten.
</commit_message>
<xml_diff>
--- a/Data/Sonntag/joined_Sonntag_coord_nn.xlsx
+++ b/Data/Sonntag/joined_Sonntag_coord_nn.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sarah\Desktop\git_folder\DataScienceProject\Data\Sonntag\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E2FB098-CD23-4CF7-8FC0-8F7EED7B4FD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64DEEAED-DAEE-43DF-8ECE-5958BEB6258B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,6 +30,28 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1036,12 +1058,14 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1167,7 +1191,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1194,9 +1218,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
@@ -1251,6 +1280,9 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{56090D2F-2F8D-4DD3-B85D-7A41649EEE98}" name="Table1" displayName="Table1" ref="A1:H189" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="A1:H189" xr:uid="{56090D2F-2F8D-4DD3-B85D-7A41649EEE98}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H189">
+    <sortCondition ref="A1:A189"/>
+  </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{4698E331-9694-4111-AA9B-D967027FEBAE}" name="Index"/>
     <tableColumn id="2" xr3:uid="{D96E1CDA-2DAA-4B6B-B47C-9926123A1DF4}" name="NEUE_NAMEN"/>
@@ -1552,10 +1584,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J189"/>
+  <dimension ref="A1:J351"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+      <selection activeCell="B351" sqref="B351"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1648,10 +1680,10 @@
       <c r="D4" t="s">
         <v>255</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="12">
         <v>16.362701650694301</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="12">
         <v>48.205781183762973</v>
       </c>
       <c r="G4" t="s">
@@ -1668,10 +1700,10 @@
       <c r="D5" t="s">
         <v>255</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="12">
         <v>16.358861594767429</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="12">
         <v>48.203592798970938</v>
       </c>
       <c r="G5" t="s">
@@ -1794,10 +1826,10 @@
       <c r="D11" t="s">
         <v>254</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="12">
         <v>16.336883553860101</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="12">
         <v>48.194919391773901</v>
       </c>
       <c r="G11" t="s">
@@ -1860,10 +1892,10 @@
       <c r="D14" t="s">
         <v>255</v>
       </c>
-      <c r="E14" s="12">
+      <c r="E14" s="15">
         <v>16.362007399610491</v>
       </c>
-      <c r="F14" s="13">
+      <c r="F14" s="17">
         <v>48.201896648067986</v>
       </c>
       <c r="G14" t="s">
@@ -1934,10 +1966,10 @@
       <c r="D19" t="s">
         <v>254</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19" s="13">
         <v>16.368694000000001</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="12">
         <v>48.200527999999998</v>
       </c>
       <c r="G19" t="s">
@@ -1986,10 +2018,10 @@
       <c r="D21" t="s">
         <v>255</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="12">
         <v>16.371866173866</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="12">
         <v>48.198245099030899</v>
       </c>
       <c r="G21" t="s">
@@ -2223,10 +2255,10 @@
       <c r="D33" t="s">
         <v>254</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="12">
         <v>16.361755237940699</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="12">
         <v>48.207964058470097</v>
       </c>
       <c r="G33" t="s">
@@ -2269,10 +2301,10 @@
       <c r="D35" t="s">
         <v>254</v>
       </c>
-      <c r="E35">
+      <c r="E35" s="12">
         <v>16.3659572122668</v>
       </c>
-      <c r="F35">
+      <c r="F35" s="12">
         <v>48.204555072124897</v>
       </c>
       <c r="G35" t="s">
@@ -2364,10 +2396,10 @@
       <c r="D39" t="s">
         <v>255</v>
       </c>
-      <c r="E39" s="7">
+      <c r="E39" s="13">
         <v>16.369026000000002</v>
       </c>
-      <c r="F39">
+      <c r="F39" s="12">
         <v>48.204306000000003</v>
       </c>
       <c r="G39" t="s">
@@ -2511,6 +2543,8 @@
       <c r="B46" t="s">
         <v>43</v>
       </c>
+      <c r="E46" s="12"/>
+      <c r="F46" s="12"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47">
@@ -2525,10 +2559,10 @@
       <c r="D47" t="s">
         <v>255</v>
       </c>
-      <c r="E47">
+      <c r="E47" s="12">
         <v>16.3673894389274</v>
       </c>
-      <c r="F47">
+      <c r="F47" s="12">
         <v>48.198865889213501</v>
       </c>
       <c r="G47" t="s">
@@ -2597,10 +2631,10 @@
       <c r="D50" t="s">
         <v>255</v>
       </c>
-      <c r="E50">
+      <c r="E50" s="12">
         <v>16.3673894389274</v>
       </c>
-      <c r="F50">
+      <c r="F50" s="12">
         <v>48.198865889213501</v>
       </c>
       <c r="G50" t="s">
@@ -2686,10 +2720,10 @@
       <c r="D54" t="s">
         <v>255</v>
       </c>
-      <c r="E54" s="14">
+      <c r="E54" s="16">
         <v>16.376831816725058</v>
       </c>
-      <c r="F54" s="15">
+      <c r="F54" s="18">
         <v>48.197382170211647</v>
       </c>
       <c r="G54" t="s">
@@ -2732,7 +2766,7 @@
       <c r="D56" t="s">
         <v>255</v>
       </c>
-      <c r="E56">
+      <c r="E56" s="12">
         <v>16.380099999999999</v>
       </c>
       <c r="F56" s="5">
@@ -2824,10 +2858,10 @@
       <c r="D60" t="s">
         <v>255</v>
       </c>
-      <c r="E60" s="12">
+      <c r="E60" s="15">
         <v>16.37795565196965</v>
       </c>
-      <c r="F60" s="13">
+      <c r="F60" s="17">
         <v>48.199667816992303</v>
       </c>
       <c r="G60" t="s">
@@ -2920,6 +2954,8 @@
       <c r="B66" t="s">
         <v>54</v>
       </c>
+      <c r="E66" s="12"/>
+      <c r="F66" s="12"/>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67">
@@ -2988,10 +3024,10 @@
       <c r="D70" t="s">
         <v>254</v>
       </c>
-      <c r="E70">
+      <c r="E70" s="12">
         <v>16.392141649460701</v>
       </c>
-      <c r="F70">
+      <c r="F70" s="12">
         <v>48.193100955666402</v>
       </c>
       <c r="G70" t="s">
@@ -3256,10 +3292,10 @@
       <c r="D83" t="s">
         <v>254</v>
       </c>
-      <c r="E83">
+      <c r="E83" s="12">
         <v>16.384374670156699</v>
       </c>
-      <c r="F83">
+      <c r="F83" s="12">
         <v>48.203154771736699</v>
       </c>
       <c r="G83" t="s">
@@ -3296,6 +3332,8 @@
       <c r="B85" t="s">
         <v>75</v>
       </c>
+      <c r="E85" s="12"/>
+      <c r="F85" s="12"/>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86">
@@ -3310,10 +3348,10 @@
       <c r="D86" t="s">
         <v>255</v>
       </c>
-      <c r="E86">
+      <c r="E86" s="12">
         <v>16.376276583298299</v>
       </c>
-      <c r="F86">
+      <c r="F86" s="12">
         <v>48.208622776513202</v>
       </c>
       <c r="G86" t="s">
@@ -3361,10 +3399,10 @@
       <c r="D89" t="s">
         <v>255</v>
       </c>
-      <c r="E89">
+      <c r="E89" s="12">
         <v>16.379973327112349</v>
       </c>
-      <c r="F89">
+      <c r="F89" s="12">
         <v>48.209980399463213</v>
       </c>
       <c r="G89" t="s">
@@ -3443,6 +3481,8 @@
       <c r="B94" t="s">
         <v>77</v>
       </c>
+      <c r="F94" s="12"/>
+      <c r="G94" s="12"/>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95">
@@ -3457,10 +3497,10 @@
       <c r="D95" t="s">
         <v>255</v>
       </c>
-      <c r="E95">
+      <c r="E95" s="12">
         <v>16.395002029909101</v>
       </c>
-      <c r="F95">
+      <c r="F95" s="12">
         <v>48.211351233037902</v>
       </c>
       <c r="G95" t="s">
@@ -3503,10 +3543,10 @@
       <c r="D97" t="s">
         <v>254</v>
       </c>
-      <c r="E97">
+      <c r="E97" s="12">
         <v>16.414195198823599</v>
       </c>
-      <c r="F97">
+      <c r="F97" s="12">
         <v>48.205516257724597</v>
       </c>
       <c r="G97" t="s">
@@ -3620,6 +3660,8 @@
       <c r="B103" t="s">
         <v>89</v>
       </c>
+      <c r="E103" s="12"/>
+      <c r="F103" s="12"/>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A104">
@@ -4146,10 +4188,10 @@
       <c r="D129" t="s">
         <v>255</v>
       </c>
-      <c r="E129">
+      <c r="E129" s="12">
         <v>16.37089487712133</v>
       </c>
-      <c r="F129">
+      <c r="F129" s="12">
         <v>48.214424546543647</v>
       </c>
       <c r="G129" t="s">
@@ -4210,6 +4252,8 @@
       <c r="B132" t="s">
         <v>80</v>
       </c>
+      <c r="F132" s="12"/>
+      <c r="G132" s="12"/>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A133">
@@ -4362,10 +4406,10 @@
       <c r="D139" t="s">
         <v>255</v>
       </c>
-      <c r="E139">
+      <c r="E139" s="12">
         <v>16.363835558603199</v>
       </c>
-      <c r="F139">
+      <c r="F139" s="12">
         <v>48.220433225640001</v>
       </c>
       <c r="G139" t="s">
@@ -4648,10 +4692,10 @@
       <c r="D153" t="s">
         <v>255</v>
       </c>
-      <c r="E153">
+      <c r="E153" s="12">
         <v>16.358228749999999</v>
       </c>
-      <c r="F153">
+      <c r="F153" s="12">
         <v>48.218601169999999</v>
       </c>
       <c r="G153" t="s">
@@ -4671,10 +4715,10 @@
       <c r="D154" t="s">
         <v>255</v>
       </c>
-      <c r="E154">
+      <c r="E154" s="12">
         <v>16.358331544138501</v>
       </c>
-      <c r="F154">
+      <c r="F154" s="12">
         <v>48.217020890050698</v>
       </c>
       <c r="G154" t="s">
@@ -4863,10 +4907,10 @@
       <c r="D164" t="s">
         <v>255</v>
       </c>
-      <c r="E164">
+      <c r="E164" s="12">
         <v>16.3627143666587</v>
       </c>
-      <c r="F164">
+      <c r="F164" s="12">
         <v>48.211441045644698</v>
       </c>
       <c r="G164" t="s">
@@ -5047,10 +5091,10 @@
       <c r="D172" t="s">
         <v>255</v>
       </c>
-      <c r="E172">
+      <c r="E172" s="12">
         <v>16.344858318868098</v>
       </c>
-      <c r="F172">
+      <c r="F172" s="12">
         <v>48.2072450727103</v>
       </c>
       <c r="G172" t="s">
@@ -5070,10 +5114,10 @@
       <c r="D173" t="s">
         <v>255</v>
       </c>
-      <c r="E173">
+      <c r="E173" s="12">
         <v>16.361304165514252</v>
       </c>
-      <c r="F173">
+      <c r="F173" s="12">
         <v>48.209892009052354</v>
       </c>
       <c r="G173" t="s">
@@ -5090,10 +5134,10 @@
       <c r="D174" t="s">
         <v>253</v>
       </c>
-      <c r="E174" s="8">
+      <c r="E174" s="14">
         <v>16.366648059999999</v>
       </c>
-      <c r="F174" s="8">
+      <c r="F174" s="14">
         <v>48.207747529999999</v>
       </c>
       <c r="G174" t="s">
@@ -5280,10 +5324,10 @@
       <c r="D182" t="s">
         <v>255</v>
       </c>
-      <c r="E182">
+      <c r="E182" s="12">
         <v>16.3644986548132</v>
       </c>
-      <c r="F182">
+      <c r="F182" s="12">
         <v>48.206795119564909</v>
       </c>
       <c r="G182" t="s">
@@ -5365,6 +5409,8 @@
       <c r="B187" t="s">
         <v>160</v>
       </c>
+      <c r="E187" s="12"/>
+      <c r="F187" s="12"/>
     </row>
     <row r="188" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A188">
@@ -5392,6 +5438,812 @@
       </c>
       <c r="B189" t="s">
         <v>162</v>
+      </c>
+    </row>
+    <row r="191" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B191" t="str" cm="1">
+        <f t="array" ref="B191:B349">_xlfn.UNIQUE(B2:B189)</f>
+        <v>k. k. Burg</v>
+      </c>
+      <c r="E191">
+        <f>COUNTA(E2:E189)</f>
+        <v>151</v>
+      </c>
+    </row>
+    <row r="192" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B192" t="str">
+        <v>Burgplatz</v>
+      </c>
+    </row>
+    <row r="193" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B193" t="str">
+        <v>Burgthor</v>
+      </c>
+    </row>
+    <row r="194" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B194" t="str">
+        <v>kaiserlichen Stallungen</v>
+      </c>
+    </row>
+    <row r="195" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B195" t="str">
+        <v>Gebäude der ungarischen Garde</v>
+      </c>
+    </row>
+    <row r="196" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B196" t="str">
+        <v>Palais des  Fürsten Auersperg</v>
+      </c>
+    </row>
+    <row r="197" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B197" t="str">
+        <v>Gebäude des Geographischen (Militär=)Jnstituts</v>
+      </c>
+    </row>
+    <row r="198" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B198" t="str">
+        <v>KriminalGebäude</v>
+      </c>
+    </row>
+    <row r="199" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B199" t="str">
+        <v>Kahlengebirge</v>
+      </c>
+    </row>
+    <row r="200" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B200" t="str">
+        <v>Mariahilfer Hauptstraße</v>
+      </c>
+    </row>
+    <row r="201" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B201" t="str">
+        <v>Schönbrunn</v>
+      </c>
+    </row>
+    <row r="202" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B202" t="str">
+        <v>Grenadierkaserne</v>
+      </c>
+    </row>
+    <row r="203" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B203" t="str">
+        <v>Getreidemarkt</v>
+      </c>
+    </row>
+    <row r="204" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B204" t="str">
+        <v>artesischen Brunnen</v>
+      </c>
+    </row>
+    <row r="205" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B205" t="str">
+        <v>Akazien=Alleen</v>
+      </c>
+    </row>
+    <row r="206" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B206" t="str">
+        <v>Wien</v>
+      </c>
+    </row>
+    <row r="207" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B207" t="str">
+        <v>Kettenstege</v>
+      </c>
+    </row>
+    <row r="208" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B208" t="str">
+        <v>der steinernen Brücke</v>
+      </c>
+    </row>
+    <row r="209" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B209" t="str">
+        <v>Polytechnische Jnstitut</v>
+      </c>
+    </row>
+    <row r="210" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B210" t="str">
+        <v>Karlskirche</v>
+      </c>
+    </row>
+    <row r="211" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B211" t="str">
+        <v>Burg</v>
+      </c>
+    </row>
+    <row r="212" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B212" t="str">
+        <v>RitterCeremoniensaal</v>
+      </c>
+    </row>
+    <row r="213" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B213" t="str">
+        <v>Appartements Sr Majestät des Kaisers</v>
+      </c>
+    </row>
+    <row r="214" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B214" t="str">
+        <v>Rittersaal</v>
+      </c>
+    </row>
+    <row r="215" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B215" t="str">
+        <v>AntikenMineralienkabinet</v>
+      </c>
+    </row>
+    <row r="216" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B216" t="str">
+        <v>astronomische Thurm</v>
+      </c>
+    </row>
+    <row r="217" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B217" t="str">
+        <v>Hofbibliotek=Gebäudes</v>
+      </c>
+    </row>
+    <row r="218" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B218" t="str">
+        <v>Josephsplatze</v>
+      </c>
+    </row>
+    <row r="219" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B219" t="str">
+        <v>Palais des  Erzherzogs Karl</v>
+      </c>
+    </row>
+    <row r="220" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B220" t="str">
+        <v>Volksgarten</v>
+      </c>
+    </row>
+    <row r="221" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B221" t="str">
+        <v>Burggarten</v>
+      </c>
+    </row>
+    <row r="222" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B222" t="str">
+        <v>Gewächshäuser</v>
+      </c>
+    </row>
+    <row r="223" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B223" t="str">
+        <v>Wall</v>
+      </c>
+    </row>
+    <row r="224" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B224" t="str">
+        <v>Spitalplatze</v>
+      </c>
+    </row>
+    <row r="225" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B225" t="str">
+        <v>Hofbauamte</v>
+      </c>
+    </row>
+    <row r="226" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B226" t="str">
+        <v>Kärnthnerthor=Theater</v>
+      </c>
+    </row>
+    <row r="227" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B227" t="str">
+        <v>Kärnthnerthore</v>
+      </c>
+    </row>
+    <row r="228" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B228" t="str">
+        <v>Kärnthnerstraße</v>
+      </c>
+    </row>
+    <row r="229" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B229" t="str">
+        <v>Wieden</v>
+      </c>
+    </row>
+    <row r="230" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B230" t="str">
+        <v>Baden</v>
+      </c>
+    </row>
+    <row r="231" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B231" t="str">
+        <v>Starhembergische Freihaus</v>
+      </c>
+    </row>
+    <row r="232" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B232" t="str">
+        <v>Wienerwaldes</v>
+      </c>
+    </row>
+    <row r="233" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B233" t="str">
+        <v>Schneeberg</v>
+      </c>
+    </row>
+    <row r="234" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B234" t="str">
+        <v>Sommerpalais des  Fürsten  Schwarzenberg</v>
+      </c>
+    </row>
+    <row r="235" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B235" t="str">
+        <v>Belvedere</v>
+      </c>
+    </row>
+    <row r="236" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B236" t="str">
+        <v>Bahnhofe</v>
+      </c>
+    </row>
+    <row r="237" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B237" t="str">
+        <v>Kirche und Kloster der Salesianerinnen</v>
+      </c>
+    </row>
+    <row r="238" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B238" t="str">
+        <v>Schwarzenbergischen Palais</v>
+      </c>
+    </row>
+    <row r="239" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B239" t="str">
+        <v>Kaserne</v>
+      </c>
+    </row>
+    <row r="240" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B240" t="str">
+        <v>Palais</v>
+      </c>
+    </row>
+    <row r="241" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B241" t="str">
+        <v>Stadtgraben</v>
+      </c>
+    </row>
+    <row r="242" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B242" t="str">
+        <v>Palais Kolowrat</v>
+      </c>
+    </row>
+    <row r="243" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B243" t="str">
+        <v>Artillerie=Haupt=Zeugamt</v>
+      </c>
+    </row>
+    <row r="244" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B244" t="str">
+        <v>Karolinenthor</v>
+      </c>
+    </row>
+    <row r="245" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B245" t="str">
+        <v>Seilerstätte</v>
+      </c>
+    </row>
+    <row r="246" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B246" t="str">
+        <v>Weihburggasse</v>
+      </c>
+    </row>
+    <row r="247" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B247" t="str">
+        <v>Mineralwässer=Trinkkur=Anstalt</v>
+      </c>
+    </row>
+    <row r="248" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B248" t="str">
+        <v>Rennweg</v>
+      </c>
+    </row>
+    <row r="249" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B249" t="str">
+        <v>Palais des Herzogs von Koburg</v>
+      </c>
+    </row>
+    <row r="250" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B250" t="str">
+        <v>orientalische Akademie</v>
+      </c>
+    </row>
+    <row r="251" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B251" t="str">
+        <v>Stubenthor</v>
+      </c>
+    </row>
+    <row r="252" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B252" t="str">
+        <v>Wollzeile</v>
+      </c>
+    </row>
+    <row r="253" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B253" t="str">
+        <v>große Steinbrücke</v>
+      </c>
+    </row>
+    <row r="254" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B254" t="str">
+        <v>Landstraße</v>
+      </c>
+    </row>
+    <row r="255" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B255" t="str">
+        <v>zur Linie (Barriere) von St. Marx</v>
+      </c>
+    </row>
+    <row r="256" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B256" t="str">
+        <v>Ungarn</v>
+      </c>
+    </row>
+    <row r="257" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B257" t="str">
+        <v>Münzgebäude</v>
+      </c>
+    </row>
+    <row r="258" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B258" t="str">
+        <v xml:space="preserve">Neustädter </v>
+      </c>
+    </row>
+    <row r="259" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B259" t="str">
+        <v>Kanal</v>
+      </c>
+    </row>
+    <row r="260" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B260" t="str">
+        <v>Stückbohrerei</v>
+      </c>
+    </row>
+    <row r="261" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B261" t="str">
+        <v>Jnvalidenhaus</v>
+      </c>
+    </row>
+    <row r="262" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B262" t="str">
+        <v>Kanalbassin</v>
+      </c>
+    </row>
+    <row r="263" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B263" t="str">
+        <v>Kloster und Kirche der  Dominikaner</v>
+      </c>
+    </row>
+    <row r="264" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B264" t="str">
+        <v>Ravelin</v>
+      </c>
+    </row>
+    <row r="265" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B265" t="str">
+        <v>Hauptmauth</v>
+      </c>
+    </row>
+    <row r="266" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B266" t="str">
+        <v>Fahrpost</v>
+      </c>
+    </row>
+    <row r="267" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B267" t="str">
+        <v>Glacis</v>
+      </c>
+    </row>
+    <row r="268" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B268" t="str">
+        <v>Zollamt</v>
+      </c>
+    </row>
+    <row r="269" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B269" t="str">
+        <v>Donaukanal</v>
+      </c>
+    </row>
+    <row r="270" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B270" t="str">
+        <v>Praters</v>
+      </c>
+    </row>
+    <row r="271" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B271" t="str">
+        <v>Leopoldstadt</v>
+      </c>
+    </row>
+    <row r="272" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B272" t="str">
+        <v>Ferdinandsbrücke</v>
+      </c>
+    </row>
+    <row r="273" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B273" t="str">
+        <v>Rothenthurm=Thore</v>
+      </c>
+    </row>
+    <row r="274" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B274" t="str">
+        <v>Taborstraße</v>
+      </c>
+    </row>
+    <row r="275" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B275" t="str">
+        <v>Tabor</v>
+      </c>
+    </row>
+    <row r="276" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B276" t="str">
+        <v>Mähren</v>
+      </c>
+    </row>
+    <row r="277" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B277" t="str">
+        <v>Böhmen</v>
+      </c>
+    </row>
+    <row r="278" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B278" t="str">
+        <v>Jägerzeile</v>
+      </c>
+    </row>
+    <row r="279" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B279" t="str">
+        <v>Donau</v>
+      </c>
+    </row>
+    <row r="280" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B280" t="str">
+        <v>Kornspeicher</v>
+      </c>
+    </row>
+    <row r="281" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B281" t="str">
+        <v>Franzensbrücke</v>
+      </c>
+    </row>
+    <row r="282" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B282" t="str">
+        <v>. Bastei</v>
+      </c>
+    </row>
+    <row r="283" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B283" t="str">
+        <v>unter den  Weißgärbern</v>
+      </c>
+    </row>
+    <row r="284" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B284" t="str">
+        <v>Erdberg</v>
+      </c>
+    </row>
+    <row r="285" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B285" t="str">
+        <v>Laurenzer=Gasse</v>
+      </c>
+    </row>
+    <row r="286" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B286" t="str">
+        <v>Laurenzerhof</v>
+      </c>
+    </row>
+    <row r="287" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B287" t="str">
+        <v>Staats=Buchhaltungen</v>
+      </c>
+    </row>
+    <row r="288" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B288" t="str">
+        <v>Müllerische Palais</v>
+      </c>
+    </row>
+    <row r="289" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B289" t="str">
+        <v>Dianabad</v>
+      </c>
+    </row>
+    <row r="290" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B290" t="str">
+        <v>Karls=Kettenbrücke</v>
+      </c>
+    </row>
+    <row r="291" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B291" t="str">
+        <v>Schanzl</v>
+      </c>
+    </row>
+    <row r="292" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B292" t="str">
+        <v>Fischmarkt</v>
+      </c>
+    </row>
+    <row r="293" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B293" t="str">
+        <v>St. Ruprechtstiege</v>
+      </c>
+    </row>
+    <row r="294" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B294" t="str">
+        <v>Fischerthore</v>
+      </c>
+    </row>
+    <row r="295" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B295" t="str">
+        <v>Salzgries</v>
+      </c>
+    </row>
+    <row r="296" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B296" t="str">
+        <v>Polizeihaus</v>
+      </c>
+    </row>
+    <row r="297" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B297" t="str">
+        <v>Stabsstockhaus</v>
+      </c>
+    </row>
+    <row r="298" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B298" t="str">
+        <v>Elendbastei</v>
+      </c>
+    </row>
+    <row r="299" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B299" t="str">
+        <v>Observatorium</v>
+      </c>
+    </row>
+    <row r="300" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B300" t="str">
+        <v>Thore</v>
+      </c>
+    </row>
+    <row r="301" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B301" t="str">
+        <v>Augartenbrücke</v>
+      </c>
+    </row>
+    <row r="302" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B302" t="str">
+        <v>Augartens</v>
+      </c>
+    </row>
+    <row r="303" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B303" t="str">
+        <v>Brigittenau</v>
+      </c>
+    </row>
+    <row r="304" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B304" t="str">
+        <v>Roßau</v>
+      </c>
+    </row>
+    <row r="305" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B305" t="str">
+        <v>Lichtenthal</v>
+      </c>
+    </row>
+    <row r="306" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B306" t="str">
+        <v>Servitenkirche</v>
+      </c>
+    </row>
+    <row r="307" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B307" t="str">
+        <v>Döbling</v>
+      </c>
+    </row>
+    <row r="308" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B308" t="str">
+        <v>Leopoldsberg</v>
+      </c>
+    </row>
+    <row r="309" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B309" t="str">
+        <v>Herzogsburg der Babenberge</v>
+      </c>
+    </row>
+    <row r="310" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B310" t="str">
+        <v>Kahlenberg</v>
+      </c>
+    </row>
+    <row r="311" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B311" t="str">
+        <v>Josephsberg</v>
+      </c>
+    </row>
+    <row r="312" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B312" t="str">
+        <v>Bastei</v>
+      </c>
+    </row>
+    <row r="313" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B313" t="str">
+        <v>Arsenales</v>
+      </c>
+    </row>
+    <row r="314" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B314" t="str">
+        <v>Proviantbäckerei</v>
+      </c>
+    </row>
+    <row r="315" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B315" t="str">
+        <v>Schottenthore</v>
+      </c>
+    </row>
+    <row r="316" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B316" t="str">
+        <v>Schottengasse</v>
+      </c>
+    </row>
+    <row r="317" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B317" t="str">
+        <v>Freiung</v>
+      </c>
+    </row>
+    <row r="318" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B318" t="str">
+        <v>Herrngasse</v>
+      </c>
+    </row>
+    <row r="319" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B319" t="str">
+        <v>Währingergasse</v>
+      </c>
+    </row>
+    <row r="320" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B320" t="str">
+        <v>Gewehrfabrik</v>
+      </c>
+    </row>
+    <row r="321" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B321" t="str">
+        <v>GarnisonsBettmagazin</v>
+      </c>
+    </row>
+    <row r="322" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B322" t="str">
+        <v>fürstlichEsterhazische sogenannte rothe Haus</v>
+      </c>
+    </row>
+    <row r="323" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B323" t="str">
+        <v>Jnfanterie=Kaserne</v>
+      </c>
+    </row>
+    <row r="324" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B324" t="str">
+        <v>Alsergasse</v>
+      </c>
+    </row>
+    <row r="325" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B325" t="str">
+        <v>Dornbach</v>
+      </c>
+    </row>
+    <row r="326" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B326" t="str">
+        <v>Kriminale</v>
+      </c>
+    </row>
+    <row r="327" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B327" t="str">
+        <v>Mölkerbastei</v>
+      </c>
+    </row>
+    <row r="328" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B328" t="str">
+        <v>Teinfaltstraße</v>
+      </c>
+    </row>
+    <row r="329" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B329" t="str">
+        <v>Palais Lubomirski</v>
+      </c>
+    </row>
+    <row r="330" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B330" t="str">
+        <v>Franzensthor</v>
+      </c>
+    </row>
+    <row r="331" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B331" t="str">
+        <v>Josephstadt</v>
+      </c>
+    </row>
+    <row r="332" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B332" t="str">
+        <v>geographische Jnstitut</v>
+      </c>
+    </row>
+    <row r="333" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B333" t="str">
+        <v>Kaisergasse</v>
+      </c>
+    </row>
+    <row r="334" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B334" t="str">
+        <v>Josephstädter Theater</v>
+      </c>
+    </row>
+    <row r="335" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B335" t="str">
+        <v>Kavallerie=Kaserne</v>
+      </c>
+    </row>
+    <row r="336" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B336" t="str">
+        <v>Lerchenfeld</v>
+      </c>
+    </row>
+    <row r="337" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B337" t="str">
+        <v>Löwelbastei</v>
+      </c>
+    </row>
+    <row r="338" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B338" t="str">
+        <v>Paradies=Gärtchen</v>
+      </c>
+    </row>
+    <row r="339" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B339" t="str">
+        <v>Cortis=Kaffehhause</v>
+      </c>
+    </row>
+    <row r="340" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B340" t="str">
+        <v>Schenkenstraße</v>
+      </c>
+    </row>
+    <row r="341" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B341" t="str">
+        <v>Palais Liechtenstein</v>
+      </c>
+    </row>
+    <row r="342" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B342" t="str">
+        <v>Staats=Kanzlei</v>
+      </c>
+    </row>
+    <row r="343" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B343" t="str">
+        <v>Ballplatz</v>
+      </c>
+    </row>
+    <row r="344" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B344" t="str">
+        <v>Bellaria</v>
+      </c>
+    </row>
+    <row r="345" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B345" t="str">
+        <v>zweites Kaffehaus von Corti</v>
+      </c>
+    </row>
+    <row r="346" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B346" t="str">
+        <v>Theseustempel</v>
+      </c>
+    </row>
+    <row r="347" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B347" t="str">
+        <v>Hof=Burgwache</v>
+      </c>
+    </row>
+    <row r="348" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B348" t="str">
+        <v>Schweizerhof</v>
+      </c>
+    </row>
+    <row r="349" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B349" t="str">
+        <v>Kunstvereine</v>
+      </c>
+    </row>
+    <row r="351" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B351">
+        <f>COUNTA(B191:B349)</f>
+        <v>159</v>
       </c>
     </row>
   </sheetData>

</xml_diff>